<commit_message>
Amendment for Sharepoint Bug
</commit_message>
<xml_diff>
--- a/EU Exit PPP Regulation Service/Documentation/Logs/EU Exit PPP-23.02.2022.xlsx
+++ b/EU Exit PPP Regulation Service/Documentation/Logs/EU Exit PPP-23.02.2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1006990\Downloads\EU-Exit-PPP-Regulation-Service\EU Exit PPP Regulation Service\Documentation\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0B187D-DBCF-4267-BF6C-50EB22B08A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14075274-A76B-4130-89C8-F849ACC1CADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="4455" windowWidth="14400" windowHeight="7365" xr2:uid="{41FE75CF-736B-4CA7-8345-FBFE6FD9683D}"/>
+    <workbookView xWindow="0" yWindow="2860" windowWidth="14400" windowHeight="7370" xr2:uid="{41FE75CF-736B-4CA7-8345-FBFE6FD9683D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="18">
   <si>
     <t>Workpackage</t>
   </si>
@@ -61,6 +61,64 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>EU Exit PPP Regulation Service</t>
+  </si>
+  <si>
+    <t>m1006990</t>
+  </si>
+  <si>
+    <t>Case 0</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Could not find the UI element corresponding to this selector:
+&lt;webctrl id='id__119' tag='SPAN'/&gt;
+The closest matches found are:
+[93%] &lt;webctrl id='id__159' tag='SPAN'/&gt;
+[86%] &lt;webctrl id='id__142' tag='SPAN'/&gt;
+[86%] &lt;webctrl id='id__147' tag='SPAN'/&gt;
+[86%] &lt;webctrl id='id__150' tag='SPAN'/&gt;
+[86%] &lt;webctrl id='id__153' tag='SPAN'/&gt;
+[86%] &lt;webctrl id='id__156' tag='SPAN'/&gt;
+[86%] &lt;webctrl id='id__186' tag='SPAN'/&gt;
+[83%] &lt;webctrl id='id__0' tag='SPAN'/&gt;
+[64%] &lt;webctrl id='header58-modifiedByColumn_1102' tag='SPAN'/&gt;
+[62%] &lt;webctrl id='header58-modifiedByColumn_1102-name' tag='SPAN'/&gt; at Source: Invoke Upload File - Amended workflow: Click 'Upload'</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Cannot send input to UI element because it is outside of screen bounds. at Source: Invoke Upload File - Amended workflow: Click 'Upload'</t>
+  </si>
+  <si>
+    <t>Could not find the user-interface (UI) element for this action._x000D_
+_x000D_
+Possible solutions:_x000D_
+ •  Ensure application is opened and the UI element is visible on the screen at execution time_x000D_
+ •  Edit the Target of the UI activity and use Validation to debug the issue. _x000D_
+ •  If needed, re-indicate the element as its properties might have changed_x000D_
+ •  Use "Check state" activity to check the application state before executing the action_x000D_
+ •  Increase the "Delay before" value to allow time to the application to render entirely and become responsive at Source: Invoke Move File - Amended workflow: Click Document to Move</t>
+  </si>
+  <si>
+    <t>Could not find the UI element corresponding to this selector:
+&lt;webctrl id='id__504' tag='SPAN'/&gt;
+The closest matches found are:
+[93%] &lt;webctrl id='id__150' tag='SPAN'/&gt;
+[92%] &lt;webctrl id='id__0' tag='SPAN'/&gt;
+[86%] &lt;webctrl id='id__142' tag='SPAN'/&gt;
+[86%] &lt;webctrl id='id__147' tag='SPAN'/&gt;
+[86%] &lt;webctrl id='id__153' tag='SPAN'/&gt;
+[86%] &lt;webctrl id='id__156' tag='SPAN'/&gt;
+[86%] &lt;webctrl id='id__159' tag='SPAN'/&gt;
+[79%] &lt;webctrl id='id__186' tag='SPAN'/&gt;
+[64%] &lt;webctrl id='header58-displayNameColumn_504' tag='SPAN'/&gt;
+[63%] &lt;webctrl id='header58-dateModifiedColumn_506' tag='SPAN'/&gt; at Source: Invoke Upload File - Amended workflow: Click 'Upload'</t>
   </si>
 </sst>
 </file>
@@ -96,8 +154,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9292166-F507-4674-B1E1-E45CF05F0FF1}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,6 +509,238 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44615.466597222221</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44615.466597222221</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44615.466597222221</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44615.470902777779</v>
+      </c>
+      <c r="E3" s="1">
+        <v>44615.470902777779</v>
+      </c>
+      <c r="F3" s="1">
+        <v>44615.470902777779</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44615.493020833332</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44615.493020833332</v>
+      </c>
+      <c r="F4" s="1">
+        <v>44615.493009259262</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44615.501631944448</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44615.501631944448</v>
+      </c>
+      <c r="F5" s="1">
+        <v>44615.501620370371</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44615.503993055558</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44615.503993055558</v>
+      </c>
+      <c r="F6" s="1">
+        <v>44615.503993055558</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44615.510810185187</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44615.510810185187</v>
+      </c>
+      <c r="F7" s="1">
+        <v>44615.510798611111</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44615.519965277781</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44615.519965277781</v>
+      </c>
+      <c r="F8" s="1">
+        <v>44615.519953703704</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44615.522592592592</v>
+      </c>
+      <c r="E9" s="1">
+        <v>44615.522592592592</v>
+      </c>
+      <c r="F9" s="1">
+        <v>44615.522592592592</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>